<commit_message>
+plot_funs, +redundant features removal
</commit_message>
<xml_diff>
--- a/xlsx/eco_manual_cleaned.xlsx
+++ b/xlsx/eco_manual_cleaned.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UBAN\R_Python_Projects\ICEF_ML\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B010A115-7DB9-4678-9C2A-B969FCA86DBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DAF7395-93B5-42DE-951B-A27CBF22E816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -793,9 +793,6 @@
     <t>[55.74743, 37.63255]</t>
   </si>
   <si>
-    <t>ГЭС-1 (Государственная электрическая станция № 1)Мосэнерго</t>
-  </si>
-  <si>
     <t>[55.518568, 37.579966]</t>
   </si>
   <si>
@@ -1319,6 +1316,9 @@
   </si>
   <si>
     <t>[55.521695, 37.526743, 55.522894, 37.521185, 55.5243, 37.521196, 55.524684, 37.521421, 55.525134, 37.522108, 55.525578, 37.524222]</t>
+  </si>
+  <si>
+    <t>тэц ГЭС-1 (Государственная электрическая станция № 1)Мосэнерго</t>
   </si>
 </sst>
 </file>
@@ -1683,8 +1683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B217"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A137" workbookViewId="0">
-      <selection activeCell="J220" sqref="J220"/>
+    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
+      <selection activeCell="B135" sqref="B135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1878,7 +1878,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B24" t="s">
         <v>46</v>
@@ -1926,7 +1926,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B30" t="s">
         <v>57</v>
@@ -1934,7 +1934,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B31" t="s">
         <v>58</v>
@@ -1942,7 +1942,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B32" t="s">
         <v>59</v>
@@ -1966,7 +1966,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B35" t="s">
         <v>64</v>
@@ -2078,7 +2078,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B49" t="s">
         <v>91</v>
@@ -2110,7 +2110,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B53" t="s">
         <v>98</v>
@@ -2582,7 +2582,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B112" t="s">
         <v>214</v>
@@ -2590,7 +2590,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B113" t="s">
         <v>215</v>
@@ -2761,671 +2761,671 @@
         <v>256</v>
       </c>
       <c r="B134" t="s">
-        <v>257</v>
+        <v>432</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
+        <v>257</v>
+      </c>
+      <c r="B135" t="s">
         <v>258</v>
-      </c>
-      <c r="B135" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
+        <v>259</v>
+      </c>
+      <c r="B136" t="s">
         <v>260</v>
-      </c>
-      <c r="B136" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
+        <v>261</v>
+      </c>
+      <c r="B137" t="s">
         <v>262</v>
-      </c>
-      <c r="B137" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
+        <v>263</v>
+      </c>
+      <c r="B138" t="s">
         <v>264</v>
-      </c>
-      <c r="B138" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
+        <v>265</v>
+      </c>
+      <c r="B139" t="s">
         <v>266</v>
-      </c>
-      <c r="B139" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
+        <v>267</v>
+      </c>
+      <c r="B140" t="s">
         <v>268</v>
-      </c>
-      <c r="B140" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
+        <v>269</v>
+      </c>
+      <c r="B141" t="s">
         <v>270</v>
-      </c>
-      <c r="B141" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
+        <v>271</v>
+      </c>
+      <c r="B142" t="s">
         <v>272</v>
-      </c>
-      <c r="B142" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
+        <v>273</v>
+      </c>
+      <c r="B143" t="s">
         <v>274</v>
-      </c>
-      <c r="B143" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
+        <v>275</v>
+      </c>
+      <c r="B144" t="s">
         <v>276</v>
-      </c>
-      <c r="B144" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
+        <v>277</v>
+      </c>
+      <c r="B145" t="s">
         <v>278</v>
-      </c>
-      <c r="B145" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
+        <v>279</v>
+      </c>
+      <c r="B146" t="s">
         <v>280</v>
-      </c>
-      <c r="B146" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
+        <v>281</v>
+      </c>
+      <c r="B147" t="s">
         <v>282</v>
-      </c>
-      <c r="B147" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
+        <v>283</v>
+      </c>
+      <c r="B148" t="s">
         <v>284</v>
-      </c>
-      <c r="B148" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
+        <v>294</v>
+      </c>
+      <c r="B149" t="s">
         <v>295</v>
-      </c>
-      <c r="B149" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B150" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B151" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
+        <v>298</v>
+      </c>
+      <c r="B152" t="s">
         <v>299</v>
-      </c>
-      <c r="B152" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B153" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B154" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B155" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B156" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B157" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B158" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B159" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B160" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
+        <v>308</v>
+      </c>
+      <c r="B161" t="s">
         <v>309</v>
-      </c>
-      <c r="B161" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B162" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
+        <v>311</v>
+      </c>
+      <c r="B163" t="s">
         <v>312</v>
-      </c>
-      <c r="B163" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
+        <v>313</v>
+      </c>
+      <c r="B164" t="s">
         <v>314</v>
-      </c>
-      <c r="B164" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
+        <v>315</v>
+      </c>
+      <c r="B165" t="s">
         <v>316</v>
-      </c>
-      <c r="B165" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B166" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B167" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
+        <v>319</v>
+      </c>
+      <c r="B168" t="s">
         <v>320</v>
-      </c>
-      <c r="B168" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B169" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B170" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
+        <v>323</v>
+      </c>
+      <c r="B171" t="s">
         <v>324</v>
-      </c>
-      <c r="B171" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
+        <v>325</v>
+      </c>
+      <c r="B172" t="s">
         <v>326</v>
-      </c>
-      <c r="B172" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
+        <v>327</v>
+      </c>
+      <c r="B173" t="s">
         <v>328</v>
-      </c>
-      <c r="B173" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
+        <v>329</v>
+      </c>
+      <c r="B174" t="s">
         <v>330</v>
-      </c>
-      <c r="B174" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
+        <v>331</v>
+      </c>
+      <c r="B175" t="s">
         <v>332</v>
-      </c>
-      <c r="B175" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
+        <v>333</v>
+      </c>
+      <c r="B176" t="s">
         <v>334</v>
-      </c>
-      <c r="B176" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
+        <v>335</v>
+      </c>
+      <c r="B177" t="s">
         <v>336</v>
-      </c>
-      <c r="B177" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
+        <v>337</v>
+      </c>
+      <c r="B178" t="s">
         <v>338</v>
-      </c>
-      <c r="B178" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
+        <v>339</v>
+      </c>
+      <c r="B179" t="s">
         <v>340</v>
-      </c>
-      <c r="B179" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
+        <v>341</v>
+      </c>
+      <c r="B180" t="s">
         <v>342</v>
-      </c>
-      <c r="B180" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
+        <v>343</v>
+      </c>
+      <c r="B181" t="s">
         <v>344</v>
-      </c>
-      <c r="B181" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
+        <v>345</v>
+      </c>
+      <c r="B182" t="s">
         <v>346</v>
-      </c>
-      <c r="B182" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
+        <v>347</v>
+      </c>
+      <c r="B183" t="s">
         <v>348</v>
-      </c>
-      <c r="B183" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
+        <v>349</v>
+      </c>
+      <c r="B184" t="s">
         <v>350</v>
-      </c>
-      <c r="B184" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
+        <v>351</v>
+      </c>
+      <c r="B185" t="s">
         <v>352</v>
-      </c>
-      <c r="B185" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
+        <v>353</v>
+      </c>
+      <c r="B186" t="s">
         <v>354</v>
-      </c>
-      <c r="B186" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
+        <v>355</v>
+      </c>
+      <c r="B187" t="s">
         <v>356</v>
-      </c>
-      <c r="B187" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
+        <v>357</v>
+      </c>
+      <c r="B188" t="s">
         <v>358</v>
-      </c>
-      <c r="B188" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
+        <v>359</v>
+      </c>
+      <c r="B189" t="s">
         <v>360</v>
-      </c>
-      <c r="B189" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
+        <v>361</v>
+      </c>
+      <c r="B190" t="s">
         <v>362</v>
-      </c>
-      <c r="B190" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
+        <v>363</v>
+      </c>
+      <c r="B191" t="s">
         <v>364</v>
-      </c>
-      <c r="B191" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
+        <v>365</v>
+      </c>
+      <c r="B192" t="s">
         <v>366</v>
-      </c>
-      <c r="B192" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
+        <v>367</v>
+      </c>
+      <c r="B193" t="s">
         <v>368</v>
-      </c>
-      <c r="B193" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
+        <v>369</v>
+      </c>
+      <c r="B194" t="s">
         <v>370</v>
-      </c>
-      <c r="B194" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B195" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
+        <v>372</v>
+      </c>
+      <c r="B196" t="s">
         <v>373</v>
-      </c>
-      <c r="B196" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
+        <v>374</v>
+      </c>
+      <c r="B197" t="s">
         <v>375</v>
-      </c>
-      <c r="B197" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
+        <v>376</v>
+      </c>
+      <c r="B198" t="s">
         <v>377</v>
-      </c>
-      <c r="B198" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
+        <v>378</v>
+      </c>
+      <c r="B199" t="s">
         <v>379</v>
-      </c>
-      <c r="B199" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
+        <v>380</v>
+      </c>
+      <c r="B200" t="s">
         <v>381</v>
-      </c>
-      <c r="B200" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
+        <v>382</v>
+      </c>
+      <c r="B201" t="s">
         <v>383</v>
-      </c>
-      <c r="B201" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
+        <v>384</v>
+      </c>
+      <c r="B202" t="s">
         <v>385</v>
-      </c>
-      <c r="B202" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
+        <v>386</v>
+      </c>
+      <c r="B203" t="s">
         <v>387</v>
-      </c>
-      <c r="B203" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
+        <v>388</v>
+      </c>
+      <c r="B204" t="s">
         <v>389</v>
-      </c>
-      <c r="B204" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
+        <v>390</v>
+      </c>
+      <c r="B205" t="s">
         <v>391</v>
-      </c>
-      <c r="B205" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B206" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
+        <v>393</v>
+      </c>
+      <c r="B207" t="s">
         <v>394</v>
-      </c>
-      <c r="B207" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
+        <v>395</v>
+      </c>
+      <c r="B208" t="s">
         <v>396</v>
-      </c>
-      <c r="B208" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
+        <v>397</v>
+      </c>
+      <c r="B209" t="s">
         <v>398</v>
-      </c>
-      <c r="B209" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B210" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B211" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
+        <v>401</v>
+      </c>
+      <c r="B212" t="s">
         <v>402</v>
-      </c>
-      <c r="B212" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
+        <v>403</v>
+      </c>
+      <c r="B213" t="s">
         <v>404</v>
-      </c>
-      <c r="B213" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B214" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B215" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B216" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B217" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
   </sheetData>

</xml_diff>